<commit_message>
More work on ACBalanceManager and CabinConfiguration: Weight and Balance modules are completed!
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
@@ -15,12 +15,13 @@
     <sheet name="NACELLES" r:id="rId9" sheetId="7"/>
     <sheet name="POWER PLANT" r:id="rId10" sheetId="8"/>
     <sheet name="LANDING GEARS" r:id="rId11" sheetId="9"/>
+    <sheet name="SYSTEMS" r:id="rId12" sheetId="10"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="73">
   <si>
     <t>Description</t>
   </si>
@@ -31,73 +32,139 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Xcg structure MAC</t>
+    <t>STRUCTURAL MASS CG</t>
+  </si>
+  <si>
+    <t>Xcg Structure BRF</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Ycg Structure BRF</t>
+  </si>
+  <si>
+    <t>Zcg Structure BRF</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Xcg Structure MAC</t>
   </si>
   <si>
     <t>%</t>
   </si>
   <si>
-    <t>Xcg structure BRF</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Zcg structure MAC</t>
-  </si>
-  <si>
-    <t>Zcg structure BRF</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Xcg structure and engines MAC</t>
-  </si>
-  <si>
-    <t>Xcg structure and engines BRF</t>
-  </si>
-  <si>
-    <t>Zcg structure and engines MAC</t>
-  </si>
-  <si>
-    <t>Zcg structure and engines BRF</t>
-  </si>
-  <si>
-    <t>Xcg operating empty mass MAC</t>
-  </si>
-  <si>
-    <t>Xcg operating empty mass BRF</t>
-  </si>
-  <si>
-    <t>Zcg operating empty mass MAC</t>
-  </si>
-  <si>
-    <t>Zcg operating empty mass BRF</t>
-  </si>
-  <si>
-    <t>Xcg maximum zero fuel mass MAC</t>
-  </si>
-  <si>
-    <t>Xcg maximum zero fuel mass BRF</t>
-  </si>
-  <si>
-    <t>Zcg maximum zero fuel mass MAC</t>
-  </si>
-  <si>
-    <t>Zcg maximum zero fuel mass BRF</t>
-  </si>
-  <si>
-    <t>Xcg maximum take-off mass MAC</t>
-  </si>
-  <si>
-    <t>Xcg maximum take-off mass BRF</t>
-  </si>
-  <si>
-    <t>Zcg maximum take-off mass MAC</t>
-  </si>
-  <si>
-    <t>Zcg maximum take-off mass BRF</t>
+    <t>Ycg Structure MAC</t>
+  </si>
+  <si>
+    <t>Zcg Structure MAC</t>
+  </si>
+  <si>
+    <t>STRUCTURAL MASS PLUS POWER PLANT CG</t>
+  </si>
+  <si>
+    <t>Xcg Structure and engines BRF</t>
+  </si>
+  <si>
+    <t>Ycg Structure and engines BRF</t>
+  </si>
+  <si>
+    <t>Zcg Structure and engines BRF</t>
+  </si>
+  <si>
+    <t>Xcg Structure and engines MAC</t>
+  </si>
+  <si>
+    <t>Ycg Structure and engines MAC</t>
+  </si>
+  <si>
+    <t>Zcg Structure and engines MAC</t>
+  </si>
+  <si>
+    <t>MANUFACTURER EMPTY MASS CG</t>
+  </si>
+  <si>
+    <t>Xcg Manufacturer empty mass BRF</t>
+  </si>
+  <si>
+    <t>Ycg Manufacturer empty mass BRF</t>
+  </si>
+  <si>
+    <t>Zcg Manufacturer empty mass BRF</t>
+  </si>
+  <si>
+    <t>Xcg Manufacturer empty mass MAC</t>
+  </si>
+  <si>
+    <t>Ycg Manufacturer empty mass MAC</t>
+  </si>
+  <si>
+    <t>Zcg Manufacturer empty mass MAC</t>
+  </si>
+  <si>
+    <t>OPERATING EMPTY MASS CG</t>
+  </si>
+  <si>
+    <t>Xcg Operating empty mass BRF</t>
+  </si>
+  <si>
+    <t>Ycg Operating empty mass BRF</t>
+  </si>
+  <si>
+    <t>Zcg Operating empty mass BRF</t>
+  </si>
+  <si>
+    <t>Xcg Operating empty mass MAC</t>
+  </si>
+  <si>
+    <t>Ycg Operating empty mass MAC</t>
+  </si>
+  <si>
+    <t>Zcg Operating empty mass MAC</t>
+  </si>
+  <si>
+    <t>MAXIMUM ZERO-FUEL MASS CG</t>
+  </si>
+  <si>
+    <t>Xcg Maximum zero fuel mass BRF</t>
+  </si>
+  <si>
+    <t>Ycg Maximum zero fuel mass BRF</t>
+  </si>
+  <si>
+    <t>Zcg Maximum zero fuel mass BRF</t>
+  </si>
+  <si>
+    <t>Xcg Maximum zero fuel mass MAC</t>
+  </si>
+  <si>
+    <t>Ycg Maximum zero fuel mass MAC</t>
+  </si>
+  <si>
+    <t>Zcg Maximum zero fuel mass MAC</t>
+  </si>
+  <si>
+    <t>MAXIMUM TAKE-OFF MASS CG</t>
+  </si>
+  <si>
+    <t>Xcg Maximum take-off mass BRF</t>
+  </si>
+  <si>
+    <t>Ycg Maximum take-off mass BRF</t>
+  </si>
+  <si>
+    <t>Zcg Maximum take-off mass BRF</t>
+  </si>
+  <si>
+    <t>Xcg Maximum take-off mass MAC</t>
+  </si>
+  <si>
+    <t>Ycg Maximum take-off mass MAC</t>
+  </si>
+  <si>
+    <t>Zcg Maximum take-off mass MAC</t>
   </si>
   <si>
     <t>Max forward Xcg MAC</t>
@@ -148,22 +215,31 @@
     <t>Ycg BRF (semi-tail)</t>
   </si>
   <si>
-    <t>BALANCE ESTIMATION FOR EACH NACELLE</t>
-  </si>
-  <si>
-    <t>NACELLE 1</t>
-  </si>
-  <si>
-    <t>NACELLE 2</t>
-  </si>
-  <si>
-    <t>BALANCE ESTIMATION FOR EACH ENGINE</t>
-  </si>
-  <si>
-    <t>ENGINE 1</t>
-  </si>
-  <si>
-    <t>ENGINE 2</t>
+    <t>TORENBEEK_1976</t>
+  </si>
+  <si>
+    <t>Zcg ESTIMATION METHOD COMPARISON</t>
+  </si>
+  <si>
+    <t>APU</t>
+  </si>
+  <si>
+    <t>AIR CONDITIONING AND ANTI-ICING SYSTEM</t>
+  </si>
+  <si>
+    <t>INSTRUMENTS AND NAVIGATION SYSTEM</t>
+  </si>
+  <si>
+    <t>HYDRAULIC AND PNEUMATIC SYSTEMS</t>
+  </si>
+  <si>
+    <t>ELECTRICAL SYSTEMS</t>
+  </si>
+  <si>
+    <t>CONTROL SURFACES</t>
+  </si>
+  <si>
+    <t>FURNISHINGS AND EQUIPMENTS</t>
   </si>
 </sst>
 </file>
@@ -250,60 +326,54 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
-        <v>25.42751997433762</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>17.52350817134971</v>
+        <v>17.0196433963224</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>-6.458493475355942</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.26052926474683</v>
+        <v>-0.5528677789553924</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
       <c r="C7" t="n">
-        <v>5.3385390034979805</v>
+        <v>28.435595869234266</v>
       </c>
     </row>
     <row r="8">
@@ -311,10 +381,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>16.713138467978993</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -322,195 +392,801 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>-10.870697395083647</v>
+        <v>-14.182417156939847</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>-0.4385132245520056</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="n">
-        <v>5.3385390034979805</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>16.713138467978993</v>
+        <v>16.127744402035546</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>-10.870697395083647</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.4385132245520056</v>
+        <v>-0.6955688214724032</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C17" t="n">
-        <v>-11.988172608583982</v>
+        <v>5.556194897936333</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C18" t="n">
-        <v>16.01419598952007</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>-8.891093938020905</v>
+        <v>-17.84304957348324</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="n">
-        <v>-0.3586579711362057</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" t="n">
-        <v>-3.95087864420811</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>16.338412510769643</v>
+        <v>15.251900498370496</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>-9.457480987175748</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.38150546676989994</v>
+        <v>-0.4593200653024182</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.13080150310339905</v>
+        <v>-16.911353544857906</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-11.782688415989861</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
         <v>27</v>
       </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="n">
+        <v>15.251900498370496</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="n">
+        <v>-0.4593200653024182</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="n">
+        <v>-16.911353544857906</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="n">
+        <v>-11.782688415989861</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="n">
+        <v>16.134885858942944</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="n">
+        <v>-0.33048903779859085</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="n">
+        <v>5.739390817149414</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" t="n">
+        <v>-8.477855968946695</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="n">
+        <v>16.271232869714964</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" t="n">
+        <v>-0.4611820512728746</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" t="n">
+        <v>9.237026704927539</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>46</v>
+      </c>
+      <c r="B58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" t="n">
+        <v>-11.830452931808235</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="n">
+        <v>-21.708800382148954</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>49</v>
+      </c>
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" t="n">
+        <v>9.237026704927539</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <cols>
+    <col min="2" max="2" width="8.0" customWidth="true"/>
+    <col min="3" max="3" width="15.0" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>30.166649999999997</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>13.854999999999997</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2.9605499999999996</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>18.67210372500307</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-0.4630372210593406</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>9.888049999999996</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-0.8624999999999998</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>0.09013194968612882</v>
+        <v>15.546879643773472</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1.7889705722583957</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="n">
+        <v>16.621649999999995</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.9249999999999998</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -543,10 +1219,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
         <v>16.988911111111108</v>
@@ -554,10 +1230,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
@@ -565,10 +1241,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -576,15 +1252,15 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
         <v>16.988911111111104</v>
@@ -592,10 +1268,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
         <v>0.0</v>
@@ -603,10 +1279,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>0.0</v>
@@ -614,20 +1290,20 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
         <v>17.143322222222217</v>
@@ -635,10 +1311,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
         <v>16.8345</v>
@@ -674,32 +1350,32 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>3.7805924820719747</v>
+        <v>3.94050072910464</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>6.135472857305533</v>
+        <v>5.556533960383371</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -707,82 +1383,104 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>16.320592482071973</v>
+        <v>16.110500729104636</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>6.135472857305532</v>
+        <v>5.55653396038337</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.43999999999999995</v>
+        <v>-0.7999999999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>3.7805924820719747</v>
+        <v>4.3629715646212155</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3.5180298935880643</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="n">
-        <v>6.135472857305533</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="n">
+        <v>4.998846772296348</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="n">
+        <v>6.114221148470394</v>
       </c>
     </row>
   </sheetData>
@@ -815,21 +1513,21 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>4.628476968600747</v>
+        <v>4.454708646856945</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
@@ -837,10 +1535,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -848,26 +1546,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>17.168476968600743</v>
+        <v>16.624708646856945</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
         <v>0.0</v>
@@ -875,18 +1573,18 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.43999999999999995</v>
+        <v>-0.7999999999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -919,32 +1617,32 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.82764988072668</v>
+        <v>1.7981052333017615</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>2.3640659711220495</v>
+        <v>2.269503332277167</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -952,37 +1650,37 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>34.577649880726675</v>
+        <v>33.39810523330176</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>2.364065971122049</v>
+        <v>2.269503332277167</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>1.0</v>
@@ -990,44 +1688,44 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>1.82764988072668</v>
+        <v>1.7981052333017615</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>2.3640659711220495</v>
+        <v>2.2695033322771674</v>
       </c>
     </row>
   </sheetData>
@@ -1060,32 +1758,32 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>3.7551851195994708</v>
+        <v>3.4971039999999975</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>2.3331999999999997</v>
+        <v>2.333199999999999</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -1093,26 +1791,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>34.50518511959946</v>
+        <v>36.49710399999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
         <v>0.0</v>
@@ -1120,55 +1818,55 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>4.183199999999999</v>
+        <v>3.8531999999999984</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>3.7551851195994708</v>
+        <v>3.4971039999999975</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>2.3331999999999997</v>
+        <v>2.3331999999999993</v>
       </c>
     </row>
   </sheetData>
@@ -1201,194 +1899,94 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1.4571999999999998</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>12.599999999999998</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>5.999999999999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-1.0999999999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="n">
-        <v>13.407199999999998</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>5.484399999999999</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.0999999999999999</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1.4571999999999998</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="n">
-        <v>13.407199999999998</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="n">
-        <v>-5.484399999999999</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="n">
-        <v>-1.0999999999999999</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>9</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -1421,194 +2019,94 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1.5919999999999996</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>13.599999999999998</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>5.999999999999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-1.0999999999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="n">
-        <v>13.541999999999998</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>5.484399999999999</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.1699999999999997</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1.5919999999999996</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="n">
-        <v>13.541999999999998</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="n">
-        <v>-5.484399999999999</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="n">
-        <v>-1.0999999999999999</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>9</v>
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>
@@ -1641,21 +2139,21 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>17.257710822429665</v>
+        <v>15.894452449346488</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
         <v>0.0</v>
@@ -1663,18 +2161,93 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.4564225053078548</v>
+        <v>-3.0364225053078546</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>15.894452449346488</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-3.036422505307854</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>15.894452449346488</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-3.0364225053078546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on aerodynamic database
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
@@ -193,10 +193,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON</t>
   </si>
   <si>
+    <t>SFORZA</t>
+  </si>
+  <si>
     <t>TORENBEEK_1982</t>
-  </si>
-  <si>
-    <t>SFORZA</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -955,7 +955,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>16.8345</v>
+        <v>17.143322222222217</v>
       </c>
     </row>
     <row r="12">
@@ -966,7 +966,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>17.143322222222217</v>
+        <v>16.8345</v>
       </c>
     </row>
   </sheetData>
@@ -1086,7 +1086,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>3.5180298935880643</v>
+        <v>4.3629715646212155</v>
       </c>
     </row>
     <row r="12">
@@ -1097,7 +1097,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>4.3629715646212155</v>
+        <v>3.5180298935880643</v>
       </c>
     </row>
     <row r="13">
@@ -1118,7 +1118,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>6.114221148470394</v>
+        <v>4.998846772296348</v>
       </c>
     </row>
     <row r="16">
@@ -1129,7 +1129,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>4.998846772296348</v>
+        <v>6.114221148470394</v>
       </c>
     </row>
   </sheetData>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -1488,7 +1488,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -1749,7 +1749,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1869,7 +1869,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
More test on Weight and Balance analyses. More work on ACPerformanceManager concerning the Descent phase.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
@@ -193,10 +193,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON</t>
   </si>
   <si>
+    <t>TORENBEEK_1982</t>
+  </si>
+  <si>
     <t>SFORZA</t>
-  </si>
-  <si>
-    <t>TORENBEEK_1982</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -955,7 +955,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>17.143322222222217</v>
+        <v>16.8345</v>
       </c>
     </row>
     <row r="12">
@@ -966,7 +966,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>16.8345</v>
+        <v>17.143322222222217</v>
       </c>
     </row>
   </sheetData>
@@ -1086,7 +1086,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>4.3629715646212155</v>
+        <v>3.5180298935880643</v>
       </c>
     </row>
     <row r="12">
@@ -1097,7 +1097,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>3.5180298935880643</v>
+        <v>4.3629715646212155</v>
       </c>
     </row>
     <row r="13">
@@ -1118,7 +1118,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>4.998846772296348</v>
+        <v>6.114221148470394</v>
       </c>
     </row>
     <row r="16">
@@ -1129,7 +1129,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>6.114221148470394</v>
+        <v>4.998846772296348</v>
       </c>
     </row>
   </sheetData>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -1488,7 +1488,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -1749,7 +1749,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1869,7 +1869,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
More work on ACAnalysisManager.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
@@ -313,7 +313,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>17.0196433963224</v>
+        <v>17.23823762216444</v>
       </c>
     </row>
     <row r="4">
@@ -335,7 +335,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.7228619316188849</v>
+        <v>-0.6999619377750967</v>
       </c>
     </row>
     <row r="6">
@@ -351,7 +351,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>28.435595869234266</v>
+        <v>34.04307493927112</v>
       </c>
     </row>
     <row r="8">
@@ -373,7 +373,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>-18.54318491929608</v>
+        <v>-17.95574380236645</v>
       </c>
     </row>
     <row r="10">
@@ -399,7 +399,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>16.127744402035546</v>
+        <v>16.40316226438204</v>
       </c>
     </row>
     <row r="14">
@@ -421,7 +421,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.8212257154737002</v>
+        <v>-0.7917816490286733</v>
       </c>
     </row>
     <row r="16">
@@ -437,7 +437,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="n">
-        <v>5.556194897936333</v>
+        <v>12.62133988368856</v>
       </c>
     </row>
     <row r="18">
@@ -459,7 +459,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>-21.066457696016553</v>
+        <v>-20.31114503534924</v>
       </c>
     </row>
     <row r="20">
@@ -485,7 +485,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>16.127744402035546</v>
+        <v>16.40316226438204</v>
       </c>
     </row>
     <row r="24">
@@ -507,7 +507,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.8212257154737002</v>
+        <v>-0.7917816490286733</v>
       </c>
     </row>
     <row r="26">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>5.556194897936333</v>
+        <v>12.62133988368856</v>
       </c>
     </row>
     <row r="28">
@@ -545,7 +545,7 @@
         <v>10</v>
       </c>
       <c r="C29" t="n">
-        <v>-21.066457696016553</v>
+        <v>-20.31114503534924</v>
       </c>
     </row>
     <row r="30">
@@ -571,7 +571,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>16.127744402035546</v>
+        <v>16.40316226438204</v>
       </c>
     </row>
     <row r="34">
@@ -593,7 +593,7 @@
         <v>5</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.8212257154737002</v>
+        <v>-0.7917816490286733</v>
       </c>
     </row>
     <row r="36">
@@ -609,7 +609,7 @@
         <v>10</v>
       </c>
       <c r="C37" t="n">
-        <v>5.556194897936333</v>
+        <v>12.62133988368856</v>
       </c>
     </row>
     <row r="38">
@@ -631,7 +631,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>-21.066457696016553</v>
+        <v>-20.31114503534924</v>
       </c>
     </row>
     <row r="40">
@@ -657,7 +657,7 @@
         <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>16.765071280503932</v>
+        <v>16.92417141603508</v>
       </c>
     </row>
     <row r="44">
@@ -679,7 +679,7 @@
         <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.5908866540451867</v>
+        <v>-0.5851922612699278</v>
       </c>
     </row>
     <row r="46">
@@ -695,7 +695,7 @@
         <v>10</v>
       </c>
       <c r="C47" t="n">
-        <v>21.90519550861985</v>
+        <v>25.986504960387446</v>
       </c>
     </row>
     <row r="48">
@@ -717,7 +717,7 @@
         <v>10</v>
       </c>
       <c r="C49" t="n">
-        <v>-15.157694731226833</v>
+        <v>-15.011619563043268</v>
       </c>
     </row>
     <row r="50">
@@ -743,7 +743,7 @@
         <v>5</v>
       </c>
       <c r="C53" t="n">
-        <v>16.725999955130618</v>
+        <v>16.840822886469397</v>
       </c>
     </row>
     <row r="54">
@@ -765,7 +765,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.6490954192088021</v>
+        <v>-0.6449790227816099</v>
       </c>
     </row>
     <row r="56">
@@ -781,7 +781,7 @@
         <v>10</v>
       </c>
       <c r="C57" t="n">
-        <v>20.902919998251257</v>
+        <v>23.848410354925875</v>
       </c>
     </row>
     <row r="58">
@@ -803,7 +803,7 @@
         <v>10</v>
       </c>
       <c r="C59" t="n">
-        <v>-16.650892600888454</v>
+        <v>-16.545296916828008</v>
       </c>
     </row>
     <row r="60">
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.43477790926796517</v>
+        <v>6.802712062372125</v>
       </c>
     </row>
     <row r="63">
@@ -835,7 +835,7 @@
         <v>10</v>
       </c>
       <c r="C63" t="n">
-        <v>25.20976261286565</v>
+        <v>29.471094089476786</v>
       </c>
     </row>
   </sheetData>
@@ -1794,7 +1794,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>15.894452449346488</v>
+        <v>16.067908020990515</v>
       </c>
     </row>
     <row r="3">
@@ -1816,7 +1816,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>-3.0364225053078546</v>
+        <v>-3.129999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -1832,7 +1832,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>15.894452449346488</v>
+        <v>16.06790802099051</v>
       </c>
     </row>
     <row r="7">
@@ -1854,7 +1854,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>-4.886422505307854</v>
+        <v>-4.979999999999999</v>
       </c>
     </row>
     <row r="9">
@@ -1875,7 +1875,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>15.894452449346488</v>
+        <v>16.067908020990515</v>
       </c>
     </row>
     <row r="12">
@@ -1896,7 +1896,7 @@
         <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>-3.0364225053078546</v>
+        <v>-3.129999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More wok on ACAnalysisManager and all other managers.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="67">
   <si>
     <t>Description</t>
   </si>
@@ -169,6 +169,9 @@
     <t>Max forward Xcg MAC</t>
   </si>
   <si>
+    <t>Operative max forward Xcg MAC</t>
+  </si>
+  <si>
     <t>Max aft Xcg MAC</t>
   </si>
   <si>
@@ -193,10 +196,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON</t>
   </si>
   <si>
+    <t>SFORZA</t>
+  </si>
+  <si>
     <t>TORENBEEK_1982</t>
-  </si>
-  <si>
-    <t>SFORZA</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -835,6 +838,17 @@
         <v>10</v>
       </c>
       <c r="C63" t="n">
+        <v>25.986504960387446</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>50</v>
+      </c>
+      <c r="B64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" t="n">
         <v>29.471094089476786</v>
       </c>
     </row>
@@ -868,7 +882,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -879,7 +893,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -890,7 +904,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -906,7 +920,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -917,7 +931,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -928,7 +942,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -944,29 +958,29 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>16.8345</v>
+        <v>17.143322222222217</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>17.143322222222217</v>
+        <v>16.8345</v>
       </c>
     </row>
   </sheetData>
@@ -999,7 +1013,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1010,7 +1024,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1021,7 +1035,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1037,7 +1051,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1048,7 +1062,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1059,7 +1073,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1075,29 +1089,29 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>3.5180298935880643</v>
+        <v>4.3629715646212155</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>4.3629715646212155</v>
+        <v>3.5180298935880643</v>
       </c>
     </row>
     <row r="13">
@@ -1107,29 +1121,29 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>6.114221148470394</v>
+        <v>4.998846772296348</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>4.998846772296348</v>
+        <v>6.114221148470394</v>
       </c>
     </row>
   </sheetData>
@@ -1162,7 +1176,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1173,7 +1187,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1184,7 +1198,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1200,7 +1214,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1211,7 +1225,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1222,7 +1236,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1266,7 +1280,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1277,7 +1291,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1288,7 +1302,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1304,7 +1318,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1315,7 +1329,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1326,7 +1340,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1342,12 +1356,12 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1363,12 +1377,12 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -1407,7 +1421,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1418,7 +1432,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1429,7 +1443,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1445,7 +1459,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1456,7 +1470,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1467,7 +1481,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1483,12 +1497,12 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1504,12 +1518,12 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -1548,7 +1562,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1559,7 +1573,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1570,7 +1584,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1586,7 +1600,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1597,7 +1611,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1608,7 +1622,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1624,12 +1638,12 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1668,7 +1682,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1679,7 +1693,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1690,7 +1704,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1706,7 +1720,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1717,7 +1731,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1728,7 +1742,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1744,7 +1758,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11">
@@ -1788,7 +1802,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1799,7 +1813,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1810,7 +1824,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1826,7 +1840,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1837,7 +1851,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1848,7 +1862,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1864,7 +1878,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11">
@@ -1885,7 +1899,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">

</xml_diff>

<commit_message>
Debugging and Add tesi Spoti
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
@@ -316,7 +316,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>17.25107428807226</v>
+        <v>17.246254408436393</v>
       </c>
     </row>
     <row r="4">
@@ -338,7 +338,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.7318532406846479</v>
+        <v>-0.7344285755648581</v>
       </c>
     </row>
     <row r="6">
@@ -354,7 +354,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>34.372366964849</v>
+        <v>34.24872520773436</v>
       </c>
     </row>
     <row r="8">
@@ -376,7 +376,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>-18.773834092229546</v>
+        <v>-18.83989776057891</v>
       </c>
     </row>
     <row r="10">
@@ -402,7 +402,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>16.412258918310712</v>
+        <v>16.411636064310827</v>
       </c>
     </row>
     <row r="14">
@@ -424,7 +424,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.9313054532297076</v>
+        <v>-0.9325556693060377</v>
       </c>
     </row>
     <row r="16">
@@ -440,7 +440,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="n">
-        <v>12.854691411231926</v>
+        <v>12.838713675522692</v>
       </c>
     </row>
     <row r="18">
@@ -462,7 +462,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>-23.89027348128807</v>
+        <v>-23.922344595948303</v>
       </c>
     </row>
     <row r="20">
@@ -488,7 +488,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>16.412258918310712</v>
+        <v>16.411636064310827</v>
       </c>
     </row>
     <row r="24">
@@ -510,7 +510,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.9313054532297076</v>
+        <v>-0.9325556693060377</v>
       </c>
     </row>
     <row r="26">
@@ -526,7 +526,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>12.854691411231926</v>
+        <v>12.838713675522692</v>
       </c>
     </row>
     <row r="28">
@@ -548,7 +548,7 @@
         <v>10</v>
       </c>
       <c r="C29" t="n">
-        <v>-23.89027348128807</v>
+        <v>-23.922344595948303</v>
       </c>
     </row>
     <row r="30">
@@ -574,7 +574,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>16.412258918310712</v>
+        <v>16.411636064310827</v>
       </c>
     </row>
     <row r="34">
@@ -596,7 +596,7 @@
         <v>5</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.9313054532297076</v>
+        <v>-0.9325556693060377</v>
       </c>
     </row>
     <row r="36">
@@ -612,7 +612,7 @@
         <v>10</v>
       </c>
       <c r="C37" t="n">
-        <v>12.854691411231926</v>
+        <v>12.838713675522692</v>
       </c>
     </row>
     <row r="38">
@@ -634,7 +634,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>-23.89027348128807</v>
+        <v>-23.922344595948303</v>
       </c>
     </row>
     <row r="40">
@@ -660,7 +660,7 @@
         <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>16.931179629317512</v>
+        <v>16.92960575115403</v>
       </c>
     </row>
     <row r="44">
@@ -682,7 +682,7 @@
         <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.6881783717369012</v>
+        <v>-0.6896245039774538</v>
       </c>
     </row>
     <row r="46">
@@ -698,7 +698,7 @@
         <v>10</v>
       </c>
       <c r="C47" t="n">
-        <v>26.16628285318501</v>
+        <v>26.12590901061653</v>
       </c>
     </row>
     <row r="48">
@@ -720,7 +720,7 @@
         <v>10</v>
       </c>
       <c r="C49" t="n">
-        <v>-17.653466376350053</v>
+        <v>-17.690563222070327</v>
       </c>
     </row>
     <row r="50">
@@ -746,7 +746,7 @@
         <v>5</v>
       </c>
       <c r="C53" t="n">
-        <v>16.84588007779047</v>
+        <v>16.82667937481264</v>
       </c>
     </row>
     <row r="54">
@@ -768,7 +768,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.8445492377297465</v>
+        <v>-0.8455920374946073</v>
       </c>
     </row>
     <row r="56">
@@ -784,7 +784,7 @@
         <v>10</v>
       </c>
       <c r="C57" t="n">
-        <v>23.978139739939795</v>
+        <v>23.485594524422805</v>
       </c>
     </row>
     <row r="58">
@@ -806,7 +806,7 @@
         <v>10</v>
       </c>
       <c r="C59" t="n">
-        <v>-21.66476335750657</v>
+        <v>-21.69151373406922</v>
       </c>
     </row>
     <row r="60">
@@ -827,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>7.019929722457434</v>
+        <v>7.0208304745943515</v>
       </c>
     </row>
     <row r="63">
@@ -838,7 +838,7 @@
         <v>10</v>
       </c>
       <c r="C63" t="n">
-        <v>26.16628285318501</v>
+        <v>26.12590901061653</v>
       </c>
     </row>
     <row r="64">
@@ -849,7 +849,7 @@
         <v>10</v>
       </c>
       <c r="C64" t="n">
-        <v>29.672168969131157</v>
+        <v>29.619176641734317</v>
       </c>
     </row>
   </sheetData>
@@ -1182,7 +1182,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>4.454708646856945</v>
+        <v>4.389801741976934</v>
       </c>
     </row>
     <row r="3">
@@ -1220,7 +1220,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>16.624708646856945</v>
+        <v>16.559801741976933</v>
       </c>
     </row>
     <row r="7">
@@ -1808,7 +1808,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>16.919871327847673</v>
+        <v>16.920581453544408</v>
       </c>
     </row>
     <row r="3">
@@ -1846,7 +1846,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>16.919871327847673</v>
+        <v>16.920581453544404</v>
       </c>
     </row>
     <row r="7">
@@ -1889,7 +1889,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>16.919871327847673</v>
+        <v>16.920581453544408</v>
       </c>
     </row>
     <row r="12">

</xml_diff>

<commit_message>
More work on AircraftCADUtils, A320neo xmls added in template aircrafts.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
@@ -257,10 +257,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
   <si>
+    <t>TORENBEEK_1982</t>
+  </si>
+  <si>
     <t>SFORZA</t>
-  </si>
-  <si>
-    <t>TORENBEEK_1982</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -1608,7 +1608,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>17.143322222222217</v>
+        <v>16.8345</v>
       </c>
     </row>
     <row r="24">
@@ -1619,7 +1619,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>16.8345</v>
+        <v>17.143322222222217</v>
       </c>
     </row>
   </sheetData>
@@ -1859,7 +1859,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>4.3631082000119275</v>
+        <v>3.5939754358446514</v>
       </c>
     </row>
     <row r="24">
@@ -1870,7 +1870,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>3.5939754358446514</v>
+        <v>4.3631082000119275</v>
       </c>
     </row>
     <row r="25">
@@ -1891,7 +1891,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>4.998846772296348</v>
+        <v>6.114221148470394</v>
       </c>
     </row>
     <row r="28">
@@ -1902,7 +1902,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>6.114221148470394</v>
+        <v>4.998846772296348</v>
       </c>
     </row>
   </sheetData>
@@ -2360,7 +2360,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2381,7 +2381,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2621,7 +2621,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2642,7 +2642,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -3122,7 +3122,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3362,7 +3362,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3383,7 +3383,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Minor bug fixes - missinf File.separator in engin import function
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
@@ -257,10 +257,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
   <si>
+    <t>TORENBEEK_1982</t>
+  </si>
+  <si>
     <t>SFORZA</t>
-  </si>
-  <si>
-    <t>TORENBEEK_1982</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -410,7 +410,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>17.536834338687946</v>
+        <v>17.536829678929287</v>
       </c>
     </row>
     <row r="4">
@@ -432,7 +432,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.7538782556948833</v>
+        <v>-0.7538730184073752</v>
       </c>
     </row>
     <row r="6">
@@ -448,7 +448,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>41.70281449477612</v>
+        <v>41.70269496051555</v>
       </c>
     </row>
     <row r="8">
@@ -470,7 +470,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>-19.338829851890605</v>
+        <v>-19.338695502595822</v>
       </c>
     </row>
     <row r="10">
@@ -496,7 +496,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>16.605757595641705</v>
+        <v>16.60575998079814</v>
       </c>
     </row>
     <row r="14">
@@ -518,7 +518,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.9539893627755958</v>
+        <v>-0.9539840868512406</v>
       </c>
     </row>
     <row r="16">
@@ -534,7 +534,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="n">
-        <v>17.8184079917303</v>
+        <v>17.818469176854272</v>
       </c>
     </row>
     <row r="18">
@@ -556,7 +556,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>-24.47217150496731</v>
+        <v>-24.472036164542455</v>
       </c>
     </row>
     <row r="20">
@@ -582,7 +582,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>15.98844740522322</v>
+        <v>15.98845144999041</v>
       </c>
     </row>
     <row r="24">
@@ -604,7 +604,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.7020194331135989</v>
+        <v>-0.702016168963008</v>
       </c>
     </row>
     <row r="26">
@@ -620,7 +620,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>1.982884618878232</v>
+        <v>1.9829883770963717</v>
       </c>
     </row>
     <row r="28">
@@ -642,7 +642,7 @@
         <v>10</v>
       </c>
       <c r="C29" t="n">
-        <v>-18.00852361392326</v>
+        <v>-18.008439880439226</v>
       </c>
     </row>
     <row r="30">
@@ -668,7 +668,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>15.98844740522322</v>
+        <v>15.98845144999041</v>
       </c>
     </row>
     <row r="34">
@@ -690,7 +690,7 @@
         <v>5</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.7020194331135989</v>
+        <v>-0.702016168963008</v>
       </c>
     </row>
     <row r="36">
@@ -706,7 +706,7 @@
         <v>10</v>
       </c>
       <c r="C37" t="n">
-        <v>1.982884618878232</v>
+        <v>1.9829883770963717</v>
       </c>
     </row>
     <row r="38">
@@ -728,7 +728,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>-18.00852361392326</v>
+        <v>-18.008439880439226</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>16.62903009618188</v>
+        <v>16.629030723969557</v>
       </c>
     </row>
     <row r="44">
@@ -776,7 +776,7 @@
         <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.5155414360990613</v>
+        <v>-0.5155397209420223</v>
       </c>
     </row>
     <row r="46">
@@ -792,7 +792,7 @@
         <v>10</v>
       </c>
       <c r="C47" t="n">
-        <v>18.415404820826627</v>
+        <v>18.415420925123296</v>
       </c>
     </row>
     <row r="48">
@@ -814,7 +814,7 @@
         <v>10</v>
       </c>
       <c r="C49" t="n">
-        <v>-13.22490473628174</v>
+        <v>-13.224860738288829</v>
       </c>
     </row>
     <row r="50">
@@ -840,7 +840,7 @@
         <v>5</v>
       </c>
       <c r="C53" t="n">
-        <v>16.609092077480064</v>
+        <v>16.609092610229034</v>
       </c>
     </row>
     <row r="54">
@@ -862,7 +862,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.6915843060147369</v>
+        <v>-0.691582512493502</v>
       </c>
     </row>
     <row r="56">
@@ -878,7 +878,7 @@
         <v>10</v>
       </c>
       <c r="C57" t="n">
-        <v>17.90394564509688</v>
+        <v>17.903959311417246</v>
       </c>
     </row>
     <row r="58">
@@ -900,7 +900,7 @@
         <v>10</v>
       </c>
       <c r="C59" t="n">
-        <v>-17.740836960377678</v>
+        <v>-17.74079095215057</v>
       </c>
     </row>
     <row r="60">
@@ -921,7 +921,7 @@
         <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>-3.410536354010929</v>
+        <v>-3.4104126235752514</v>
       </c>
     </row>
     <row r="63">
@@ -932,7 +932,7 @@
         <v>10</v>
       </c>
       <c r="C63" t="n">
-        <v>17.90394564509688</v>
+        <v>17.903959311417246</v>
       </c>
     </row>
     <row r="64">
@@ -943,7 +943,7 @@
         <v>10</v>
       </c>
       <c r="C64" t="n">
-        <v>21.146475249897982</v>
+        <v>21.146482032033443</v>
       </c>
     </row>
     <row r="65">
@@ -974,7 +974,7 @@
         <v>53</v>
       </c>
       <c r="C69" t="n">
-        <v>67806.97027432358</v>
+        <v>67807.11435421702</v>
       </c>
     </row>
     <row r="70">
@@ -985,7 +985,7 @@
         <v>53</v>
       </c>
       <c r="C70" t="n">
-        <v>923364.8355985356</v>
+        <v>923365.6135190843</v>
       </c>
     </row>
     <row r="71">
@@ -996,7 +996,7 @@
         <v>53</v>
       </c>
       <c r="C71" t="n">
-        <v>1268971.6267490634</v>
+        <v>1268972.2786296117</v>
       </c>
     </row>
     <row r="72">
@@ -1039,7 +1039,7 @@
         <v>53</v>
       </c>
       <c r="C76" t="n">
-        <v>102390.51152197254</v>
+        <v>102390.56001072339</v>
       </c>
     </row>
   </sheetData>
@@ -1608,7 +1608,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>17.143322222222217</v>
+        <v>16.8345</v>
       </c>
     </row>
     <row r="24">
@@ -1619,7 +1619,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>16.8345</v>
+        <v>17.143322222222217</v>
       </c>
     </row>
   </sheetData>
@@ -1859,7 +1859,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>4.3631082000119275</v>
+        <v>3.5939754358446514</v>
       </c>
     </row>
     <row r="24">
@@ -1870,7 +1870,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>3.5939754358446514</v>
+        <v>4.3631082000119275</v>
       </c>
     </row>
     <row r="25">
@@ -1891,7 +1891,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>4.998846772296348</v>
+        <v>6.114221148470394</v>
       </c>
     </row>
     <row r="28">
@@ -1902,7 +1902,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>6.114221148470394</v>
+        <v>4.998846772296348</v>
       </c>
     </row>
   </sheetData>
@@ -2360,7 +2360,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2381,7 +2381,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2621,7 +2621,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2642,7 +2642,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -3122,7 +3122,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3194,7 +3194,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>13.436189431353645</v>
+        <v>13.436213092549476</v>
       </c>
     </row>
     <row r="6">
@@ -3205,7 +3205,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>13.436189431353599</v>
+        <v>13.436213092549432</v>
       </c>
     </row>
     <row r="7">
@@ -3216,7 +3216,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>16.434927234669914</v>
+        <v>16.43492815704532</v>
       </c>
     </row>
     <row r="8">
@@ -3227,7 +3227,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>16.434927234669914</v>
+        <v>16.43492815704532</v>
       </c>
     </row>
     <row r="9">
@@ -3238,7 +3238,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>16.434927234669914</v>
+        <v>16.43492815704532</v>
       </c>
     </row>
     <row r="10">
@@ -3249,7 +3249,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>16.434927234669914</v>
+        <v>16.43492815704532</v>
       </c>
     </row>
     <row r="11">
@@ -3362,13 +3362,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>16.434927234669914</v>
+        <v>16.43492815704532</v>
       </c>
     </row>
     <row r="24">
@@ -3383,7 +3383,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
[JPADCAD] minor changes in sandbox inputs
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
@@ -257,10 +257,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
   <si>
+    <t>SFORZA</t>
+  </si>
+  <si>
     <t>TORENBEEK_1982</t>
-  </si>
-  <si>
-    <t>SFORZA</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -1608,7 +1608,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>16.8345</v>
+        <v>17.143322222222217</v>
       </c>
     </row>
     <row r="24">
@@ -1619,7 +1619,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>17.143322222222217</v>
+        <v>16.8345</v>
       </c>
     </row>
   </sheetData>
@@ -1859,7 +1859,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>3.5939754358446514</v>
+        <v>4.3631082000119275</v>
       </c>
     </row>
     <row r="24">
@@ -1870,7 +1870,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>4.3631082000119275</v>
+        <v>3.5939754358446514</v>
       </c>
     </row>
     <row r="25">
@@ -1891,7 +1891,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>6.114221148470394</v>
+        <v>4.998846772296348</v>
       </c>
     </row>
     <row r="28">
@@ -1902,7 +1902,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>4.998846772296348</v>
+        <v>6.114221148470394</v>
       </c>
     </row>
   </sheetData>
@@ -2360,7 +2360,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2381,7 +2381,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2621,7 +2621,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2642,7 +2642,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -3122,7 +3122,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3362,7 +3362,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3383,7 +3383,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
More work on ACAerodynamicAndStabilityManager_v2.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
@@ -15,13 +15,12 @@
     <sheet name="NACELLES" r:id="rId9" sheetId="7"/>
     <sheet name="POWER PLANT" r:id="rId10" sheetId="8"/>
     <sheet name="LANDING GEARS" r:id="rId11" sheetId="9"/>
-    <sheet name="SYSTEMS" r:id="rId12" sheetId="10"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="89">
   <si>
     <t>Description</t>
   </si>
@@ -288,33 +287,6 @@
   </si>
   <si>
     <t>Zcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
-  </si>
-  <si>
-    <t>APU</t>
-  </si>
-  <si>
-    <t>Xcg BRF</t>
-  </si>
-  <si>
-    <t>Zcg BRF</t>
-  </si>
-  <si>
-    <t>AIR CONDITIONING AND ANTI-ICING SYSTEM</t>
-  </si>
-  <si>
-    <t>INSTRUMENTS AND NAVIGATION SYSTEM</t>
-  </si>
-  <si>
-    <t>HYDRAULIC AND PNEUMATIC SYSTEMS</t>
-  </si>
-  <si>
-    <t>ELECTRICAL SYSTEMS</t>
-  </si>
-  <si>
-    <t>CONTROL SURFACES</t>
-  </si>
-  <si>
-    <t>FURNISHINGS AND EQUIPMENTS</t>
   </si>
 </sst>
 </file>
@@ -410,7 +382,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>17.536829678929287</v>
+        <v>17.509083171496854</v>
       </c>
     </row>
     <row r="4">
@@ -432,7 +404,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.7538730184073752</v>
+        <v>-0.7618846114845372</v>
       </c>
     </row>
     <row r="6">
@@ -448,7 +420,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>41.70269496051555</v>
+        <v>40.990928860131916</v>
       </c>
     </row>
     <row r="8">
@@ -470,7 +442,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>-19.338695502595822</v>
+        <v>-19.54421255285085</v>
       </c>
     </row>
     <row r="10">
@@ -496,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>16.60575998079814</v>
+        <v>16.602082538926844</v>
       </c>
     </row>
     <row r="14">
@@ -518,7 +490,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.9539840868512406</v>
+        <v>-0.9563473932163205</v>
       </c>
     </row>
     <row r="16">
@@ -534,7 +506,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="n">
-        <v>17.818469176854272</v>
+        <v>17.724133755846978</v>
       </c>
     </row>
     <row r="18">
@@ -556,7 +528,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>-24.472036164542455</v>
+        <v>-24.532660780436228</v>
       </c>
     </row>
     <row r="20">
@@ -582,7 +554,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>15.98845144999041</v>
+        <v>16.602082538926844</v>
       </c>
     </row>
     <row r="24">
@@ -604,7 +576,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.702016168963008</v>
+        <v>-0.9563473932163205</v>
       </c>
     </row>
     <row r="26">
@@ -620,7 +592,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>1.9829883770963717</v>
+        <v>17.724133755846978</v>
       </c>
     </row>
     <row r="28">
@@ -642,7 +614,7 @@
         <v>10</v>
       </c>
       <c r="C29" t="n">
-        <v>-18.008439880439226</v>
+        <v>-24.532660780436228</v>
       </c>
     </row>
     <row r="30">
@@ -668,7 +640,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>15.98845144999041</v>
+        <v>16.602082538926844</v>
       </c>
     </row>
     <row r="34">
@@ -690,7 +662,7 @@
         <v>5</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.702016168963008</v>
+        <v>-0.9563473932163205</v>
       </c>
     </row>
     <row r="36">
@@ -706,7 +678,7 @@
         <v>10</v>
       </c>
       <c r="C37" t="n">
-        <v>1.9829883770963717</v>
+        <v>17.724133755846978</v>
       </c>
     </row>
     <row r="38">
@@ -728,7 +700,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>-18.008439880439226</v>
+        <v>-24.532660780436228</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>16.629030723969557</v>
+        <v>17.04956453589054</v>
       </c>
     </row>
     <row r="44">
@@ -776,7 +748,7 @@
         <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.5155397209420223</v>
+        <v>-0.6732119944890558</v>
       </c>
     </row>
     <row r="46">
@@ -792,7 +764,7 @@
         <v>10</v>
       </c>
       <c r="C47" t="n">
-        <v>18.415420925123296</v>
+        <v>29.20314662787694</v>
       </c>
     </row>
     <row r="48">
@@ -814,7 +786,7 @@
         <v>10</v>
       </c>
       <c r="C49" t="n">
-        <v>-13.224860738288829</v>
+        <v>-17.269542021311445</v>
       </c>
     </row>
     <row r="50">
@@ -840,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="C53" t="n">
-        <v>16.609092610229034</v>
+        <v>16.956380611370676</v>
       </c>
     </row>
     <row r="54">
@@ -862,7 +834,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.691582512493502</v>
+        <v>-0.7799135731491034</v>
       </c>
     </row>
     <row r="56">
@@ -878,7 +850,7 @@
         <v>10</v>
       </c>
       <c r="C57" t="n">
-        <v>17.903959311417246</v>
+        <v>26.812749972172895</v>
       </c>
     </row>
     <row r="58">
@@ -900,7 +872,7 @@
         <v>10</v>
       </c>
       <c r="C59" t="n">
-        <v>-17.74079095215057</v>
+        <v>-20.00669972422566</v>
       </c>
     </row>
     <row r="60">
@@ -921,7 +893,7 @@
         <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>-3.4104126235752514</v>
+        <v>11.997784147183046</v>
       </c>
     </row>
     <row r="63">
@@ -932,7 +904,7 @@
         <v>10</v>
       </c>
       <c r="C63" t="n">
-        <v>17.903959311417246</v>
+        <v>26.812749972172895</v>
       </c>
     </row>
     <row r="64">
@@ -943,7 +915,7 @@
         <v>10</v>
       </c>
       <c r="C64" t="n">
-        <v>21.146482032033443</v>
+        <v>32.8363585964546</v>
       </c>
     </row>
     <row r="65">
@@ -974,7 +946,7 @@
         <v>53</v>
       </c>
       <c r="C69" t="n">
-        <v>67807.11435421702</v>
+        <v>60154.70017136331</v>
       </c>
     </row>
     <row r="70">
@@ -985,7 +957,7 @@
         <v>53</v>
       </c>
       <c r="C70" t="n">
-        <v>923365.6135190843</v>
+        <v>3037072.693850185</v>
       </c>
     </row>
     <row r="71">
@@ -996,7 +968,7 @@
         <v>53</v>
       </c>
       <c r="C71" t="n">
-        <v>1268972.2786296117</v>
+        <v>2976917.9936788203</v>
       </c>
     </row>
     <row r="72">
@@ -1039,336 +1011,7 @@
         <v>53</v>
       </c>
       <c r="C76" t="n">
-        <v>102390.56001072339</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="70"/>
-  <cols>
-    <col min="2" max="2" width="8.0" customWidth="true"/>
-    <col min="3" max="3" width="15.0" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>30.166649999999997</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="n">
-        <v>13.854999999999997</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="n">
-        <v>-1.25</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="n">
-        <v>2.9605499999999996</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="n">
-        <v>18.630445741393828</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="n">
-        <v>-0.8219576584168198</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="n">
-        <v>9.888049999999996</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>91</v>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="n">
-        <v>-1.0874999999999997</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" t="n">
-        <v>15.441116935869058</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>84</v>
-      </c>
-      <c r="B29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" t="n">
-        <v>1.4976030710651973</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" t="n">
-        <v>16.621649999999995</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" t="n">
-        <v>0.9249999999999998</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>8</v>
+        <v>-6986.489026558615</v>
       </c>
     </row>
   </sheetData>
@@ -3194,7 +2837,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>13.436213092549476</v>
+        <v>13.534850162764503</v>
       </c>
     </row>
     <row r="6">
@@ -3205,7 +2848,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>13.436213092549432</v>
+        <v>13.534850162764458</v>
       </c>
     </row>
     <row r="7">
@@ -3216,7 +2859,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>16.43492815704532</v>
+        <v>16.43877328847313</v>
       </c>
     </row>
     <row r="8">
@@ -3227,7 +2870,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>16.43492815704532</v>
+        <v>16.43877328847313</v>
       </c>
     </row>
     <row r="9">
@@ -3238,7 +2881,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>16.43492815704532</v>
+        <v>16.43877328847313</v>
       </c>
     </row>
     <row r="10">
@@ -3249,7 +2892,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>16.43492815704532</v>
+        <v>16.43877328847313</v>
       </c>
     </row>
     <row r="11">
@@ -3368,7 +3011,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>16.43492815704532</v>
+        <v>16.43877328847313</v>
       </c>
     </row>
     <row r="24">

</xml_diff>

<commit_message>
More tests on performance
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/CS300/BALANCE/Balance.xlsx
@@ -256,10 +256,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
   <si>
+    <t>SFORZA</t>
+  </si>
+  <si>
     <t>TORENBEEK_1982</t>
-  </si>
-  <si>
-    <t>SFORZA</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -1251,7 +1251,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>16.8345</v>
+        <v>17.143322222222217</v>
       </c>
     </row>
     <row r="24">
@@ -1262,7 +1262,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>17.143322222222217</v>
+        <v>16.8345</v>
       </c>
     </row>
   </sheetData>
@@ -1502,7 +1502,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>3.5939754358446514</v>
+        <v>4.3631082000119275</v>
       </c>
     </row>
     <row r="24">
@@ -1513,7 +1513,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>4.3631082000119275</v>
+        <v>3.5939754358446514</v>
       </c>
     </row>
     <row r="25">
@@ -1534,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>6.114221148470394</v>
+        <v>4.998846772296348</v>
       </c>
     </row>
     <row r="28">
@@ -1545,7 +1545,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>4.998846772296348</v>
+        <v>6.114221148470394</v>
       </c>
     </row>
   </sheetData>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>

</xml_diff>